<commit_message>
added "messages per museum"
</commit_message>
<xml_diff>
--- a/data/analysis/temporal_analysis/museum_activity_groups_var1_accreditation.xlsx
+++ b/data/analysis/temporal_analysis/museum_activity_groups_var1_accreditation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>msg_count_twitter</t>
   </si>
@@ -22,6 +22,9 @@
     <t>msg_count_facebook</t>
   </si>
   <si>
+    <t>sum</t>
+  </si>
+  <si>
     <t>mean</t>
   </si>
   <si>
@@ -44,6 +47,9 @@
   </si>
   <si>
     <t>count</t>
+  </si>
+  <si>
+    <t>msg_per_mus</t>
   </si>
   <si>
     <t>active_mus_n</t>
@@ -419,13 +425,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:27">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -440,11 +446,11 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -453,8 +459,12 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:27">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -490,190 +500,226 @@
         <v>12</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="Z2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:27">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:27">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4">
+        <v>3321036</v>
+      </c>
+      <c r="C4">
         <v>2011.5</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>5267.7</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
       <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>471</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1765</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>75337</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1651</v>
       </c>
-      <c r="J4">
+      <c r="K4">
+        <v>2011.5</v>
+      </c>
+      <c r="L4">
         <v>1240</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>75.09999999999999</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>0.7</v>
       </c>
-      <c r="M4">
+      <c r="O4">
+        <v>766527</v>
+      </c>
+      <c r="P4">
         <v>464.3</v>
       </c>
-      <c r="N4">
+      <c r="Q4">
         <v>1048.9</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
       <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
         <v>615</v>
       </c>
-      <c r="S4">
+      <c r="V4">
         <v>13530</v>
       </c>
-      <c r="T4">
+      <c r="W4">
         <v>1651</v>
       </c>
-      <c r="U4">
+      <c r="X4">
+        <v>464.3</v>
+      </c>
+      <c r="Y4">
         <v>731</v>
       </c>
-      <c r="V4">
+      <c r="Z4">
         <v>44.3</v>
       </c>
-      <c r="W4">
+      <c r="AA4">
         <v>0.7</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:27">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5">
+        <v>2292591</v>
+      </c>
+      <c r="C5">
         <v>1358.2</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>4794.8</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>19.5</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>737.5</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>74189</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>1688</v>
       </c>
-      <c r="J5">
+      <c r="K5">
+        <v>1358.2</v>
+      </c>
+      <c r="L5">
         <v>959</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>56.8</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>-0.7</v>
       </c>
-      <c r="M5">
+      <c r="O5">
+        <v>701065</v>
+      </c>
+      <c r="P5">
         <v>415.3</v>
       </c>
-      <c r="N5">
+      <c r="Q5">
         <v>1896.8</v>
       </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
       <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
         <v>241.5</v>
       </c>
-      <c r="S5">
+      <c r="V5">
         <v>37660</v>
       </c>
-      <c r="T5">
+      <c r="W5">
         <v>1688</v>
       </c>
-      <c r="U5">
+      <c r="X5">
+        <v>415.3</v>
+      </c>
+      <c r="Y5">
         <v>518</v>
       </c>
-      <c r="V5">
+      <c r="Z5">
         <v>30.7</v>
       </c>
-      <c r="W5">
+      <c r="AA5">
         <v>-0.7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="B1:N1"/>
+    <mergeCell ref="O1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>